<commit_message>
v2p15. Compatible with MF-Swift v2306, passenger density parameterized.
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/Body/Human/sm_car_data_DriverHuman.xlsx
+++ b/Libraries/Vehicle/Body/Human/sm_car_data_DriverHuman.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Others\smiller\ssvt\Libraries\Vehicle\Body\Human\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\simscape\demo\allsimscape\cars\vehicle-templates\Libraries\Vehicle\Body\Human\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AAFA1C-9CFE-4B90-A59E-8D6CA5203C4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C219D9E-895E-460D-8ADC-7E38B904B40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1152" windowWidth="23040" windowHeight="10212" tabRatio="747" activeTab="4" xr2:uid="{06440896-8E0F-4240-830D-6ADD843B9DCF}"/>
+    <workbookView xWindow="3510" yWindow="510" windowWidth="21600" windowHeight="15210" tabRatio="747" activeTab="4" xr2:uid="{06440896-8E0F-4240-830D-6ADD843B9DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="None" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="39">
   <si>
     <t>Units</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>Truck_Amandla</t>
+  </si>
+  <si>
+    <t>rho</t>
+  </si>
+  <si>
+    <t>kg/m^3</t>
+  </si>
+  <si>
+    <t>Use to adjust passenger mass</t>
   </si>
 </sst>
 </file>
@@ -209,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -218,29 +227,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -602,28 +604,28 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AB9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="K22" sqref="K22"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -643,170 +645,165 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
-      <c r="U4"/>
-      <c r="V4"/>
-      <c r="W4"/>
-      <c r="X4"/>
-      <c r="Y4"/>
-      <c r="Z4"/>
-      <c r="AA4"/>
-      <c r="AB4"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="9">
         <v>-1.26656038245259</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="9">
         <v>0.37676294844659303</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <v>0.62577262194716998</v>
       </c>
       <c r="K5" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="9"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
       <c r="D6" t="s">
         <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="9">
         <v>0</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <v>0</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>0</v>
       </c>
-      <c r="L6" s="9"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9">
+        <v>1000</v>
+      </c>
+      <c r="K7" s="9"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11">
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9">
         <v>15</v>
       </c>
-      <c r="L7" s="9"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="10"/>
-      <c r="D8" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="8"/>
+      <c r="D9" t="s">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>0.79210000000000003</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G9" s="9">
         <v>0.8196</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H9" s="9">
         <v>0.93330000000000002</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="9"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="10"/>
-      <c r="D9" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="8"/>
+      <c r="D10" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9">
         <v>1</v>
       </c>
-      <c r="L9" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:B4">
@@ -824,7 +821,7 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AB9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
@@ -834,18 +831,18 @@
       <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -865,170 +862,165 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
-      <c r="U4"/>
-      <c r="V4"/>
-      <c r="W4"/>
-      <c r="X4"/>
-      <c r="Y4"/>
-      <c r="Z4"/>
-      <c r="AA4"/>
-      <c r="AB4"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="9">
         <v>-1.26656038245259</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="9">
         <v>0.37676294844659303</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <v>0.62577262194716998</v>
       </c>
       <c r="K5" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="9"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
       <c r="D6" t="s">
         <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="9">
         <v>0</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <v>0</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>0</v>
       </c>
-      <c r="L6" s="9"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9">
+        <v>1000</v>
+      </c>
+      <c r="K7" s="9"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11">
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9">
         <v>15</v>
       </c>
-      <c r="L7" s="9"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="10"/>
-      <c r="D8" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="8"/>
+      <c r="D9" t="s">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>0.79210000000000003</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G9" s="9">
         <v>0.8196</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H9" s="9">
         <v>0.93330000000000002</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="9"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="10"/>
-      <c r="D9" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="8"/>
+      <c r="D10" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9">
         <v>1</v>
       </c>
-      <c r="L9" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:B4">
@@ -1046,7 +1038,7 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AB22"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
@@ -1056,18 +1048,18 @@
       <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1087,244 +1079,239 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
-      <c r="U4"/>
-      <c r="V4"/>
-      <c r="W4"/>
-      <c r="X4"/>
-      <c r="Y4"/>
-      <c r="Z4"/>
-      <c r="AA4"/>
-      <c r="AB4"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="9">
         <v>-1.5695403824525895</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="9">
         <v>0.45176294844659298</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <v>0.59172262194716996</v>
       </c>
       <c r="K5" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="9"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
       <c r="D6" t="s">
         <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="9">
         <v>0</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <v>0</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>0</v>
       </c>
-      <c r="L6" s="9"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9">
+        <v>1000</v>
+      </c>
+      <c r="K7" s="9"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11">
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9">
         <v>15</v>
       </c>
-      <c r="L7" s="9"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="10"/>
-      <c r="D8" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="8"/>
+      <c r="D9" t="s">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>0.79210000000000003</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G9" s="9">
         <v>0.8196</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H9" s="9">
         <v>0.93330000000000002</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="9"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="10"/>
-      <c r="D9" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="8"/>
+      <c r="D10" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9">
         <v>1</v>
       </c>
-      <c r="L9" s="9"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="K14" s="11">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K15" s="9">
         <v>-1.3243331220516996</v>
       </c>
-      <c r="L14" s="11">
+      <c r="L15" s="9">
         <v>0.45175517503754498</v>
       </c>
-      <c r="M14" s="11">
+      <c r="M15" s="9">
         <v>0.88921153885340298</v>
       </c>
-      <c r="O14" t="s">
+      <c r="O15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="K16" s="12">
+    <row r="17" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K17" s="10">
         <v>-1.0213531220517</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L17" s="10">
         <v>0.37675517503754502</v>
       </c>
-      <c r="M16" s="12">
+      <c r="M17" s="10">
         <v>0.92326153885340301</v>
       </c>
-      <c r="O16" t="s">
+      <c r="O17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K18" s="15">
-        <f>K14-K16</f>
+    <row r="19" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K19" s="12">
+        <f>K15-K17</f>
         <v>-0.30297999999999958</v>
       </c>
-      <c r="L18" s="15">
-        <f>L14-L16</f>
+      <c r="L19" s="12">
+        <f>L15-L17</f>
         <v>7.4999999999999956E-2</v>
       </c>
-      <c r="M18" s="15">
-        <f>M14-M16</f>
+      <c r="M19" s="12">
+        <f>M15-M17</f>
         <v>-3.4050000000000025E-2</v>
       </c>
-      <c r="O18" t="s">
+      <c r="O19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K21" s="11">
+    <row r="22" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K22" s="9">
         <v>-1.26656038245259</v>
       </c>
-      <c r="L21" s="11">
+      <c r="L22" s="9">
         <v>0.37676294844659303</v>
       </c>
-      <c r="M21" s="11">
+      <c r="M22" s="9">
         <v>0.62577262194716998</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K22" s="15">
-        <f>K21+K18</f>
+    <row r="23" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K23" s="12">
+        <f>K22+K19</f>
         <v>-1.5695403824525895</v>
       </c>
-      <c r="L22" s="15">
-        <f>L21+L18</f>
+      <c r="L23" s="12">
+        <f>L22+L19</f>
         <v>0.45176294844659298</v>
       </c>
-      <c r="M22" s="15">
-        <f>M21+M18</f>
+      <c r="M23" s="12">
+        <f>M22+M19</f>
         <v>0.59172262194716996</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O23" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1344,7 +1331,7 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AB29"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
@@ -1354,18 +1341,18 @@
       <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1385,315 +1372,310 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
-      <c r="U4"/>
-      <c r="V4"/>
-      <c r="W4"/>
-      <c r="X4"/>
-      <c r="Y4"/>
-      <c r="Z4"/>
-      <c r="AA4"/>
-      <c r="AB4"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="9">
         <v>0.83</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="9">
         <v>0.55927294844659303</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <v>1.1399999999999999</v>
       </c>
-      <c r="L5" s="9"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
       <c r="D6" t="s">
         <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="9">
         <v>0</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <v>25</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>0</v>
       </c>
-      <c r="L6" s="9"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9">
+        <v>1000</v>
+      </c>
+      <c r="K7" s="9"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11">
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9">
         <v>0</v>
       </c>
-      <c r="L7" s="9"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="10"/>
-      <c r="D8" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="8"/>
+      <c r="D9" t="s">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>0.79210000000000003</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G9" s="9">
         <v>0.8196</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H9" s="9">
         <v>0.93330000000000002</v>
       </c>
-      <c r="K8" s="11"/>
-      <c r="L8" s="9"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="10"/>
-      <c r="D9" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="8"/>
+      <c r="D10" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9">
         <v>1</v>
       </c>
-      <c r="L9" s="9"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="K14" s="11">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K15" s="9">
         <v>-1.3243331220516996</v>
       </c>
-      <c r="L14" s="11">
+      <c r="L15" s="9">
         <v>0.45175517503754498</v>
       </c>
-      <c r="M14" s="11">
+      <c r="M15" s="9">
         <v>0.88921153885340298</v>
       </c>
-      <c r="O14" t="s">
+      <c r="O15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="K16" s="12">
+    <row r="17" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K17" s="10">
         <v>-1.0213531220517</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L17" s="10">
         <v>0.37675517503754502</v>
       </c>
-      <c r="M16" s="12">
+      <c r="M17" s="10">
         <v>0.92326153885340301</v>
       </c>
-      <c r="O16" t="s">
+      <c r="O17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K18" s="15">
-        <f>K14-K16</f>
+    <row r="19" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K19" s="12">
+        <f>K15-K17</f>
         <v>-0.30297999999999958</v>
       </c>
-      <c r="L18" s="15">
-        <f>L14-L16</f>
+      <c r="L19" s="12">
+        <f>L15-L17</f>
         <v>7.4999999999999956E-2</v>
       </c>
-      <c r="M18" s="15">
-        <f>M14-M16</f>
+      <c r="M19" s="12">
+        <f>M15-M17</f>
         <v>-3.4050000000000025E-2</v>
       </c>
-      <c r="O18" t="s">
+      <c r="O19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K21" s="11">
+    <row r="22" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K22" s="9">
         <v>-1.26656038245259</v>
       </c>
-      <c r="L21" s="11">
+      <c r="L22" s="9">
         <v>0.37676294844659303</v>
       </c>
-      <c r="M21" s="11">
+      <c r="M22" s="9">
         <v>0.62577262194716998</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K22" s="15">
-        <f>K21+K18</f>
+    <row r="23" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K23" s="12">
+        <f>K22+K19</f>
         <v>-1.5695403824525895</v>
       </c>
-      <c r="L22" s="15">
-        <f>L21+L18</f>
+      <c r="L23" s="12">
+        <f>L22+L19</f>
         <v>0.45176294844659298</v>
       </c>
-      <c r="M22" s="15">
-        <f>M21+M18</f>
+      <c r="M23" s="12">
+        <f>M22+M19</f>
         <v>0.59172262194716996</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K24" s="12">
+    <row r="25" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K25" s="10">
         <v>1.1638776779483</v>
       </c>
-      <c r="L24" s="12">
+      <c r="L25" s="10">
         <v>0.55926517503754503</v>
       </c>
-      <c r="M24" s="12">
+      <c r="M25" s="10">
         <v>1.3352423388534029</v>
       </c>
-      <c r="O24" t="s">
+      <c r="O25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K25" s="12">
+    <row r="26" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K26" s="10">
         <v>-1.0213531220517</v>
       </c>
-      <c r="L25" s="12">
+      <c r="L26" s="10">
         <v>0.37675517503754502</v>
       </c>
-      <c r="M25" s="12">
+      <c r="M26" s="10">
         <v>0.92326153885340301</v>
       </c>
-      <c r="O25" t="s">
+      <c r="O26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K26">
-        <f>K24-K25</f>
+    <row r="27" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <f>K25-K26</f>
         <v>2.1852308000000003</v>
       </c>
-      <c r="L26">
-        <f>L24-L25</f>
+      <c r="L27">
+        <f>L25-L26</f>
         <v>0.18251000000000001</v>
       </c>
-      <c r="M26">
-        <f>M24-M25</f>
+      <c r="M27">
+        <f>M25-M26</f>
         <v>0.41198079999999992</v>
       </c>
-      <c r="O26" t="s">
+      <c r="O27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K28" s="11">
+    <row r="29" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K29" s="9">
         <v>-1.26656038245259</v>
       </c>
-      <c r="L28" s="11">
+      <c r="L29" s="9">
         <v>0.37676294844659303</v>
       </c>
-      <c r="M28" s="11">
+      <c r="M29" s="9">
         <v>0.62577262194716998</v>
       </c>
-      <c r="O28" t="s">
+      <c r="O29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K29" s="15">
-        <f>K28+K26</f>
+    <row r="30" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K30" s="12">
+        <f>K29+K27</f>
         <v>0.9186704175474103</v>
       </c>
-      <c r="L29" s="15">
-        <f>L28+L26</f>
+      <c r="L30" s="12">
+        <f>L29+L27</f>
         <v>0.55927294844659303</v>
       </c>
-      <c r="M29" s="15">
-        <f>M28+M26</f>
+      <c r="M30" s="12">
+        <f>M29+M27</f>
         <v>1.03775342194717</v>
       </c>
-      <c r="O29" t="s">
+      <c r="O30" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1713,28 +1695,28 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AB29"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="N10" sqref="N10"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1754,315 +1736,310 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
-      <c r="U4"/>
-      <c r="V4"/>
-      <c r="W4"/>
-      <c r="X4"/>
-      <c r="Y4"/>
-      <c r="Z4"/>
-      <c r="AA4"/>
-      <c r="AB4"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="9">
         <v>-1.3230999999999999</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="9">
         <v>0.55801299999999998</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <v>2.3923999999999999</v>
       </c>
-      <c r="L5" s="9"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
       <c r="D6" t="s">
         <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="9">
         <v>0</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <v>25</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>0</v>
       </c>
-      <c r="L6" s="9"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9">
+        <v>1000</v>
+      </c>
+      <c r="K7" s="9"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11">
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9">
         <v>0</v>
       </c>
-      <c r="L7" s="9"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="10"/>
-      <c r="D8" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="8"/>
+      <c r="D9" t="s">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>0.79210000000000003</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G9" s="9">
         <v>0.8196</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H9" s="9">
         <v>0.93330000000000002</v>
       </c>
-      <c r="K8" s="11"/>
-      <c r="L8" s="9"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="10"/>
-      <c r="D9" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="8"/>
+      <c r="D10" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9">
         <v>1</v>
       </c>
-      <c r="L9" s="9"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="K14" s="11">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K15" s="9">
         <v>-1.3243331220516996</v>
       </c>
-      <c r="L14" s="11">
+      <c r="L15" s="9">
         <v>0.45175517503754498</v>
       </c>
-      <c r="M14" s="11">
+      <c r="M15" s="9">
         <v>0.88921153885340298</v>
       </c>
-      <c r="O14" t="s">
+      <c r="O15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="K16" s="12">
+    <row r="17" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K17" s="10">
         <v>-1.0213531220517</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L17" s="10">
         <v>0.37675517503754502</v>
       </c>
-      <c r="M16" s="12">
+      <c r="M17" s="10">
         <v>0.92326153885340301</v>
       </c>
-      <c r="O16" t="s">
+      <c r="O17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K18" s="15">
-        <f>K14-K16</f>
+    <row r="19" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K19" s="12">
+        <f>K15-K17</f>
         <v>-0.30297999999999958</v>
       </c>
-      <c r="L18" s="15">
-        <f>L14-L16</f>
+      <c r="L19" s="12">
+        <f>L15-L17</f>
         <v>7.4999999999999956E-2</v>
       </c>
-      <c r="M18" s="15">
-        <f>M14-M16</f>
+      <c r="M19" s="12">
+        <f>M15-M17</f>
         <v>-3.4050000000000025E-2</v>
       </c>
-      <c r="O18" t="s">
+      <c r="O19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K21" s="11">
+    <row r="22" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K22" s="9">
         <v>-1.26656038245259</v>
       </c>
-      <c r="L21" s="11">
+      <c r="L22" s="9">
         <v>0.37676294844659303</v>
       </c>
-      <c r="M21" s="11">
+      <c r="M22" s="9">
         <v>0.62577262194716998</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K22" s="15">
-        <f>K21+K18</f>
+    <row r="23" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K23" s="12">
+        <f>K22+K19</f>
         <v>-1.5695403824525895</v>
       </c>
-      <c r="L22" s="15">
-        <f>L21+L18</f>
+      <c r="L23" s="12">
+        <f>L22+L19</f>
         <v>0.45176294844659298</v>
       </c>
-      <c r="M22" s="15">
-        <f>M21+M18</f>
+      <c r="M23" s="12">
+        <f>M22+M19</f>
         <v>0.59172262194716996</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K24" s="12">
+    <row r="25" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K25" s="10">
         <v>1.1638776779483</v>
       </c>
-      <c r="L24" s="12">
+      <c r="L25" s="10">
         <v>0.55926517503754503</v>
       </c>
-      <c r="M24" s="12">
+      <c r="M25" s="10">
         <v>1.3352423388534029</v>
       </c>
-      <c r="O24" t="s">
+      <c r="O25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K25" s="12">
+    <row r="26" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K26" s="10">
         <v>-1.0213531220517</v>
       </c>
-      <c r="L25" s="12">
+      <c r="L26" s="10">
         <v>0.37675517503754502</v>
       </c>
-      <c r="M25" s="12">
+      <c r="M26" s="10">
         <v>0.92326153885340301</v>
       </c>
-      <c r="O25" t="s">
+      <c r="O26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K26">
-        <f>K24-K25</f>
+    <row r="27" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <f>K25-K26</f>
         <v>2.1852308000000003</v>
       </c>
-      <c r="L26">
-        <f>L24-L25</f>
+      <c r="L27">
+        <f>L25-L26</f>
         <v>0.18251000000000001</v>
       </c>
-      <c r="M26">
-        <f>M24-M25</f>
+      <c r="M27">
+        <f>M25-M26</f>
         <v>0.41198079999999992</v>
       </c>
-      <c r="O26" t="s">
+      <c r="O27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K28" s="11">
+    <row r="29" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K29" s="9">
         <v>-1.26656038245259</v>
       </c>
-      <c r="L28" s="11">
+      <c r="L29" s="9">
         <v>0.37676294844659303</v>
       </c>
-      <c r="M28" s="11">
+      <c r="M29" s="9">
         <v>0.62577262194716998</v>
       </c>
-      <c r="O28" t="s">
+      <c r="O29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="11:15" x14ac:dyDescent="0.3">
-      <c r="K29" s="15">
-        <f>K28+K26</f>
+    <row r="30" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K30" s="12">
+        <f>K29+K27</f>
         <v>0.9186704175474103</v>
       </c>
-      <c r="L29" s="15">
-        <f>L28+L26</f>
+      <c r="L30" s="12">
+        <f>L29+L27</f>
         <v>0.55927294844659303</v>
       </c>
-      <c r="M29" s="15">
-        <f>M28+M26</f>
+      <c r="M30" s="12">
+        <f>M29+M27</f>
         <v>1.03775342194717</v>
       </c>
-      <c r="O29" t="s">
+      <c r="O30" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>